<commit_message>
Removed 1.2000000002 error from deleted strain input test sheets.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
         <v>0.8</v>
       </c>
       <c r="D1" s="12">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="E1" s="13">
         <v>1.6</v>
@@ -1025,7 +1025,7 @@
         <v>0.8</v>
       </c>
       <c r="D1" s="9">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="E1" s="9">
         <v>1.6</v>
@@ -1401,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
wrapping up test file audit
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>CIN5</t>
   </si>
@@ -71,9 +76,6 @@
     <t>fix_b</t>
   </si>
   <si>
-    <t>Sheet</t>
-  </si>
-  <si>
     <t>estimate_params</t>
   </si>
   <si>
@@ -101,9 +103,6 @@
     <t>MM</t>
   </si>
   <si>
-    <t>targets/regulators</t>
-  </si>
-  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -116,13 +115,13 @@
     <t>DCIN5</t>
   </si>
   <si>
-    <t>Deletion</t>
+    <t>cols regulators/rows targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -175,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -183,7 +182,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -195,7 +193,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -270,6 +268,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -596,31 +597,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.64453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -629,7 +630,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -638,7 +639,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -648,7 +649,7 @@
       <c r="D4" s="5"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -658,94 +659,94 @@
       <c r="D5" s="5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="B6" s="4"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="B7" s="4"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8" s="4"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9" s="4"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10" s="4"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11" s="4"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12" s="4"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14" s="4"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15" s="4"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16" s="4"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17" s="4"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18" s="4"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20" s="4"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22"/>
       <c r="G22"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D24" s="5"/>
     </row>
   </sheetData>
@@ -757,29 +758,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.64453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -787,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -795,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -803,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -811,71 +812,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22"/>
     </row>
@@ -888,112 +889,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="B1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.64453125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="10">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9">
         <v>0.4</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="10">
         <v>0.8</v>
       </c>
-      <c r="D1" s="12">
+      <c r="D1" s="11">
         <v>1.2</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="12">
         <v>1.6</v>
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>-1.2174432654761544</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>-0.64984386018298912</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>0.26929382132237512</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>0.41593537248224854</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>0.49751163358969142</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>0.54159993841241572</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>-0.29093615522070321</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>-0.57977180156386388</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>-0.85583465653557034</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>-1.1097262320569594</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
     </row>
   </sheetData>
@@ -1005,131 +1006,131 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9">
+        <v>18</v>
+      </c>
+      <c r="B1" s="8">
         <v>0.4</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="8">
         <v>0.8</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="8">
         <v>1.2</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="8">
         <v>1.6</v>
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>-1.2174432654761544</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>-0.64984386018298912</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>-0.40259011361710589</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E7" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E22" s="2"/>
     </row>
   </sheetData>
@@ -1140,36 +1141,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.76171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.87890625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.64453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>25</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1184,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1261,35 +1262,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.76171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.87890625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.64453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.1171875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>25</v>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1321,7 +1324,7 @@
       <c r="U1"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1398,19 +1401,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1466,59 +1469,59 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="8">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7">
         <v>0.4</v>
       </c>
       <c r="C14">
@@ -1531,47 +1534,25 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
         <v>0.1</v>
       </c>
     </row>
@@ -1584,24 +1565,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>19</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1633,10 +1614,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commented out code using MM and refactored tests accordingly.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235942B-A229-4048-B9CA-7862D059395F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -100,9 +101,6 @@
     <t>expression_timepoints</t>
   </si>
   <si>
-    <t>MM</t>
-  </si>
-  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -116,6 +114,9 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1292,7 +1293,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1404,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -1471,15 +1472,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1539,10 +1540,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "Commented out code using MM and refactored tests accordingly."
This reverts commit 94f18ef5a44dfd856b4b03368d70b7cefd7e1579.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235942B-A229-4048-B9CA-7862D059395F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -101,6 +100,9 @@
     <t>expression_timepoints</t>
   </si>
   <si>
+    <t>MM</t>
+  </si>
+  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -114,9 +116,6 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
-  </si>
-  <si>
-    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1170,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1293,7 +1292,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1405,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -1472,15 +1471,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1540,10 +1539,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1569,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactored tests for MM.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235942B-A229-4048-B9CA-7862D059395F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -100,9 +101,6 @@
     <t>expression_timepoints</t>
   </si>
   <si>
-    <t>MM</t>
-  </si>
-  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -116,6 +114,9 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1292,7 +1293,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1404,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -1471,15 +1472,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1539,10 +1540,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "Refactored tests for MM."
This reverts commit 18e8f644578bbb6d78368d3346132241b1c26e9d.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235942B-A229-4048-B9CA-7862D059395F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -101,6 +100,9 @@
     <t>expression_timepoints</t>
   </si>
   <si>
+    <t>MM</t>
+  </si>
+  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -114,9 +116,6 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
-  </si>
-  <si>
-    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1170,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1293,7 +1292,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1405,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -1472,15 +1471,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1540,10 +1539,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1569,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactored code to disable MM.
</commit_message>
<xml_diff>
--- a/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
+++ b/test_files/deleted_strains_tests/deletion_parameter_ignored_test_sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GRNmap\test_files\deleted_strains_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235942B-A229-4048-B9CA-7862D059395F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -100,9 +101,6 @@
     <t>expression_timepoints</t>
   </si>
   <si>
-    <t>MM</t>
-  </si>
-  <si>
     <t>production_function</t>
   </si>
   <si>
@@ -116,6 +114,9 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1292,7 +1293,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1404,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -1471,15 +1472,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1539,10 +1540,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>